<commit_message>
added new data for Adm. de Tribunales
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_148_SoliGrupEdad.xlsx
+++ b/data/administracion_de_tribunales/OP_148_SoliGrupEdad.xlsx
@@ -1,45 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BA8EDD-749D-4C9A-851D-B47481AF7B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="4" r:id="rId1"/>
     <sheet name="2021-2022" sheetId="1" r:id="rId2"/>
     <sheet name="2022-2023" sheetId="2" r:id="rId3"/>
     <sheet name="2023-2024" sheetId="3" r:id="rId4"/>
+    <sheet name="2024-2025" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="23">
   <si>
     <t>Región</t>
   </si>
@@ -108,15 +97,12 @@
   </si>
   <si>
     <t>Cantidad total</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 20 años o menos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,9 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,22 +424,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +447,7 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -478,319 +467,265 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>15</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>35</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>25</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>24</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>9</v>
       </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1">
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>24</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>17</v>
       </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>10</v>
       </c>
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
         <v>4</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:I12" si="0">SUM(B2:B11)</f>
+        <v>134</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B13" s="1">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>3</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <f t="shared" ref="B15:I15" si="0">SUM(B2:B14)</f>
-        <v>162</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="E15">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>10</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -800,19 +735,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,9 +775,10 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -861,8 +797,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3">
@@ -875,8 +811,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4">
@@ -895,8 +831,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5">
@@ -924,8 +860,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6">
@@ -953,8 +889,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -979,8 +915,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8">
@@ -999,8 +935,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9">
@@ -1016,8 +952,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10">
@@ -1036,8 +972,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11">
@@ -1053,8 +989,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12">
@@ -1076,8 +1012,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13">
@@ -1105,8 +1041,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14">
@@ -1119,8 +1055,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15">
@@ -1163,24 +1099,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1208,9 +1144,10 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -1226,8 +1163,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3">
@@ -1243,8 +1180,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4">
@@ -1260,8 +1197,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5">
@@ -1283,8 +1220,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6">
@@ -1306,8 +1243,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -1326,8 +1263,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8">
@@ -1346,8 +1283,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9">
@@ -1366,8 +1303,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10">
@@ -1383,8 +1320,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11">
@@ -1397,8 +1334,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12">
@@ -1423,8 +1360,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13">
@@ -1452,8 +1389,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14">
@@ -1472,8 +1409,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15">
@@ -1516,20 +1453,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1557,9 +1494,10 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -1581,8 +1519,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3">
@@ -1598,8 +1536,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4">
@@ -1624,8 +1562,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5">
@@ -1647,8 +1585,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6">
@@ -1673,8 +1611,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -1699,8 +1637,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8">
@@ -1722,8 +1660,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9">
@@ -1745,8 +1683,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10">
@@ -1768,8 +1706,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11">
@@ -1779,8 +1717,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12">
@@ -1802,8 +1740,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13">
@@ -1831,8 +1769,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14">
@@ -1854,8 +1792,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B15">
@@ -1889,6 +1827,305 @@
       <c r="I15">
         <f t="shared" si="0"/>
         <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>109</v>
+      </c>
+      <c r="C15">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>